<commit_message>
Updated PPTX and Logos directories.
</commit_message>
<xml_diff>
--- a/Excel Terminado.xlsx
+++ b/Excel Terminado.xlsx
@@ -330,7 +330,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="D9:AA36"/>
+  <dimension ref="D9:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -346,33 +346,32 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>44076</v>
+        <v>44116</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K9" t="n">
         <v>1</v>
       </c>
-      <c r="L9">
-        <f>IF(N9=3, 750, IF(N9=1, 1000, ""))</f>
-        <v/>
+      <c r="L9" t="n">
+        <v>500</v>
       </c>
       <c r="M9">
         <f>L9*4</f>
@@ -388,7 +387,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>http://www.panama24horas.com.pa/panama/panama-pacifico-clave-para-la-reactivacion-economica-del-pais/</t>
+          <t>https://www.instagram.com/p/CGQouMGn-FB/?igshid=1femxospxoxhy</t>
         </is>
       </c>
     </row>
@@ -400,32 +399,33 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>44076</v>
+        <v>44117</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K10" t="n">
         <v>2</v>
       </c>
-      <c r="L10" t="n">
-        <v>500</v>
+      <c r="L10">
+        <f>IF(N10=3, 750, IF(N10=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M10">
         <f>L10*4</f>
@@ -441,7 +441,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>https://twitter.com/Panama24horas/status/1301252247108624384?s=20</t>
+          <t>https://riducaonline.com/2020/10/13/la-inteligencia-artificial-mejora-el-nivel-de-seguridad-de-las-actividades-comerciales/</t>
         </is>
       </c>
     </row>
@@ -453,11 +453,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>44077</v>
+        <v>44133</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
@@ -471,7 +471,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Zona Panamá Pacífico «clave para la reactivación económica del país»</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K11" t="n">
@@ -495,7 +495,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>https://verpanama.com/zona-panama-pacifico-2020-clave-de-reactivacion/</t>
+          <t>https://somosimpactopositivo.com/impacto-social/inteligencia-artificial/</t>
         </is>
       </c>
     </row>
@@ -507,11 +507,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>44078</v>
+        <v>44125</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>La Zona Del Pacífico Es Clave Para La Reactivación Económica Del País</t>
+          <t>Hoy en Encuentro E&amp;N Por qué invertir en seguridad biométrica para impulsar el comercio</t>
         </is>
       </c>
       <c r="K12" t="n">
@@ -549,7 +549,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>https://dpanama.com.pa/index.php/2020/09/04/la-zona-del-pacifico-es-clave-para-la-reactivacion-economica-del-pais/</t>
+          <t>https://www.estrategiaynegocios.net/tecnologia/1417011-330/encuentro-en-por-qu%C3%A9-invertir-en-seguridad-biom%C3%A9trica-para-impulsar-el-comercio</t>
         </is>
       </c>
     </row>
@@ -561,33 +561,32 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>44081</v>
+        <v>44120</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Panamá Pacífico reinicia operaciones bajo estrictos protocolos de bioseguridad</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
-      <c r="L13">
-        <f>IF(N13=3, 750, IF(N13=1, 1000, ""))</f>
-        <v/>
+      <c r="L13" t="n">
+        <v>500</v>
       </c>
       <c r="M13">
         <f>L13*4</f>
@@ -603,7 +602,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>http://www.radiomiapanama.com/noticias/noticias-nacionales/27654-panama-pacifico-reinicia-operaciones-bajo-estrictos-protocolos-de-bioseguridad.html</t>
+          <t>https://twitter.com/escenariosv/status/1317126121473847297?s=20</t>
         </is>
       </c>
     </row>
@@ -615,11 +614,11 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>44081</v>
+        <v>44134</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
@@ -633,7 +632,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Panamá Pacífico reinicia operaciones bajo estrictos protocolos de bioseguridad</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K14" t="n">
@@ -656,7 +655,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>https://twitter.com/radiomiapanama/status/1303135582948855809?s=20</t>
+          <t>https://twitter.com/Revista_EyN/status/1322289764817608705?s=20</t>
         </is>
       </c>
     </row>
@@ -668,33 +667,32 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>44081</v>
+        <v>44134</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Panamá Pacífico reinicia operaciones bajo estrictos protocolos de bioseguridad</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K15" t="n">
         <v>7</v>
       </c>
-      <c r="L15">
-        <f>IF(N15=3, 750, IF(N15=1, 1000, ""))</f>
-        <v/>
+      <c r="L15" t="n">
+        <v>500</v>
       </c>
       <c r="M15">
         <f>L15*4</f>
@@ -710,7 +708,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>https://ensegundos.com.pa/2020/09/07/panama-pacifico-reinicia-operaciones-bajo-estrictos-protocolos-de-bioseguridad/</t>
+          <t>https://twitter.com/Revista_EyN/status/1322288871401525252?s=20</t>
         </is>
       </c>
     </row>
@@ -722,11 +720,11 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>44081</v>
+        <v>44134</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
@@ -740,7 +738,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Panamá Pacífico reinicia operaciones bajo estrictos protocolos de bioseguridad</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K16" t="n">
@@ -763,7 +761,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>https://twitter.com/ensegundos_pa/status/1302995762742210562?s=20</t>
+          <t>https://twitter.com/Revista_EyN/status/1322287805700153345?s=20</t>
         </is>
       </c>
     </row>
@@ -775,33 +773,32 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica del país</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>44084</v>
+        <v>44134</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Panamá Pacífico, clave para la reactivación económica de Panamá</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K17" t="n">
         <v>9</v>
       </c>
-      <c r="L17">
-        <f>IF(N17=3, 750, IF(N17=1, 1000, ""))</f>
-        <v/>
+      <c r="L17" t="n">
+        <v>500</v>
       </c>
       <c r="M17">
         <f>L17*4</f>
@@ -817,45 +814,44 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>https://www.revistainversionesynegocios.com/2020/09/10/panama-pacifico-clave-para-la-reactivacion-economica-de-panama/</t>
+          <t>https://twitter.com/Revista_EyN/status/1322233109199392769?s=20</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
         <is>
-          <t>Nota de Prensa 2 (Agosto)</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>TRAIL, una nueva oportunidad para educarse con estándares internacionales en Panamá Pacífico</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>44077</v>
+        <v>44134</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>TRAIL, una nueva oportunidad para educarse con estándares internacionales en Panamá Pacífico</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K18" t="n">
         <v>10</v>
       </c>
-      <c r="L18">
-        <f>IF(N18=3, 750, IF(N18=1, 1000, ""))</f>
-        <v/>
+      <c r="L18" t="n">
+        <v>500</v>
       </c>
       <c r="M18">
         <f>L18*4</f>
@@ -871,35 +867,45 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>http://prnoticiaspanama.com/trail-una-nueva-oportunidad-para-educarse-con-estandares-internacionales-en-panama-pacifico/</t>
+          <t>https://twitter.com/Revista_EyN/status/1322287311762108417?s=20</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
         <is>
-          <t>Mención de Marca y Vocero</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Panamá Pacífico Juramentó su nueva junta directiva   https://www.telemetro.com/nacionales/2020/09/06/nueva-directiva-asociacion-empresas-panama/3205350.html</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>44080</v>
-      </c>
-      <c r="G19" s="2" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+        <v>44134</v>
+      </c>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Nueva directiva de la Asociación de Empresas de Panamá Pacífico toma posesión</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K19" t="n">
         <v>11</v>
       </c>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>500</v>
+      </c>
       <c r="M19">
         <f>L19*4</f>
         <v/>
@@ -914,35 +920,45 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>No Metro Libre</t>
+          <t>https://twitter.com/Revista_EyN/status/1322286505566605313?s=20</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mención de Marca y Vocero</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Panamá Pacífico Juramentó su nueva junta directiva   https://www.telemetro.com/nacionales/2020/09/06/nueva-directiva-asociacion-empresas-panama/3205350.html</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>44081</v>
-      </c>
-      <c r="G20" s="2" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+        <v>44134</v>
+      </c>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Panamá Pacífico Juramentó su nueva junta directiva</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K20" t="n">
         <v>12</v>
       </c>
-      <c r="L20" t="inlineStr"/>
+      <c r="L20" t="n">
+        <v>500</v>
+      </c>
       <c r="M20">
         <f>L20*4</f>
         <v/>
@@ -957,45 +973,44 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>No Metro Libre</t>
+          <t>https://twitter.com/Revista_EyN/status/1322284348918370306?s=20</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
         <is>
-          <t>Mención de Marca y Vocero</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Kemmy Almengor, Panamá Pacífico. Nos sentimos muy optimistas. Durante la emergencia algunas empresas no pararon sus operaciones, ya que forman parte del engranaje logístico que mantuvo funcionando al país.</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>44081</v>
+        <v>44134</v>
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Kemmy Almengor, Panamá Pacífico. Nos sentimos muy optimistas. Durante la emergencia algunas empresas no pararon sus operaciones, ya que forman parte del engranaje logístico que mantuvo funcionando al país.</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K21" t="n">
         <v>13</v>
       </c>
-      <c r="L21">
-        <f>IF(N21=3, 750, IF(N21=1, 1000, ""))</f>
-        <v/>
+      <c r="L21" t="n">
+        <v>500</v>
       </c>
       <c r="M21">
         <f>L21*4</f>
@@ -1011,45 +1026,44 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>https://riducaonline.com/2020/09/22/vivir-en-espacios-abiertos-es-la-alternativa-que-prefieren-los-usuarios-de-plataformas-digitales/</t>
+          <t>https://twitter.com/Revista_EyN/status/1322283203885998081?s=20</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="D22" t="inlineStr">
         <is>
-          <t>Nota de Prensa 3</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Vivir en espacios abiertos, es la alternativa que prefieren los usuarios de plataformas digitales luego de la pandemia</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>44096</v>
+        <v>44134</v>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Vivir en espacios abiertos, es la alternativa que prefieren los usuarios de plataformas digitales</t>
+          <t>Inteligencia artificial mejora el nivel de seguridad de las actividades comerciales</t>
         </is>
       </c>
       <c r="K22" t="n">
         <v>14</v>
       </c>
-      <c r="L22">
-        <f>IF(N22=3, 750, IF(N22=1, 1000, ""))</f>
-        <v/>
+      <c r="L22" t="n">
+        <v>500</v>
       </c>
       <c r="M22">
         <f>L22*4</f>
@@ -1065,45 +1079,35 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>https://www.elespectadordepanama.com/vivir-en-espacios-abiertos-la-alternativa-que-prefieren-los-usuarios-de-plataformas-digitales-luego-de-la-pandemia/</t>
+          <t>https://twitter.com/Revista_EyN/status/1322288058688032769?s=20</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>Nota de Prensa 3</t>
+          <t>Entrevista 1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Vivir en espacios abiertos, es la alternativa que prefieren los usuarios de plataformas digitales luego de la pandemia</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>44097</v>
-      </c>
-      <c r="G23" s="2" t="inlineStr">
-        <is>
-          <t>Twitter</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>1 post</t>
-        </is>
-      </c>
+        <v>44124</v>
+      </c>
+      <c r="G23" s="2" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Vivir en espacios abiertos, es la alternativa que prefieren los usuarios de plataformas digitales luego de la pandemia</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="K23" t="n">
         <v>15</v>
       </c>
-      <c r="L23" t="n">
-        <v>500</v>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23">
         <f>L23*4</f>
         <v/>
@@ -1118,35 +1122,46 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>https://www.telemetro.com/entrevistas/2020/09/04/gerentes-de-panama-pacifico-expresan-optimismo-ante-reapertura-el-lunes/3198871.html?utm_content=buffer6c58b&amp;utm_medium=social&amp;utm_source=twitter.com&amp;utm_campaign=app+buffer+/</t>
+          <t>No Nextv</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="D24" t="inlineStr">
         <is>
-          <t>Entrevista 1</t>
+          <t>Entrevista 2</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>44169</v>
-      </c>
-      <c r="G24" s="2" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
+        <v>44124</v>
+      </c>
+      <c r="G24" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="K24" t="n">
         <v>16</v>
       </c>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24">
+        <f>IF(N24=3, 750, IF(N24=1, 1000, ""))</f>
+        <v/>
+      </c>
       <c r="M24">
         <f>L24*4</f>
         <v/>
@@ -1161,44 +1176,45 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>No Telemetro</t>
+          <t>https://www.youtube.com/watch?v=9uCtTNO9D_o&amp;feature=youtu.be</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="D25" t="inlineStr">
         <is>
-          <t>Entrevista 1</t>
+          <t>Entrevista 3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>44078</v>
+        <v>44124</v>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="K25" t="n">
         <v>17</v>
       </c>
-      <c r="L25" t="n">
-        <v>500</v>
+      <c r="L25">
+        <f>IF(N25=3, 750, IF(N25=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M25">
         <f>L25*4</f>
@@ -1214,44 +1230,45 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>https://twitter.com/TReporta/status/1301704419218784258?s=20</t>
+          <t>https://pa.domiplay.net/video/entrevista-al-ing-enrique-luna-20-10-20-nex-9ucdo</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="D26" t="inlineStr">
         <is>
-          <t>Entrevista 1</t>
+          <t>Entrevista 4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>44077</v>
+        <v>44124</v>
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="K26" t="n">
         <v>18</v>
       </c>
-      <c r="L26" t="n">
-        <v>500</v>
+      <c r="L26">
+        <f>IF(N26=3, 750, IF(N26=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M26">
         <f>L26*4</f>
@@ -1267,44 +1284,45 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>https://twitter.com/TReporta/status/1301894476735148032?s=20</t>
+          <t>https://nexnoticias.ruplayers.com/n6d62Lixg2l4l6M/entrevista-al-ing-enrique-luna-sobre-la-inteligencia-artificial.html</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="D27" t="inlineStr">
         <is>
-          <t>Entrevista 1</t>
+          <t>Entrevista 5</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>44078</v>
+        <v>44124</v>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="K27" t="n">
         <v>19</v>
       </c>
-      <c r="L27" t="n">
-        <v>500</v>
+      <c r="L27">
+        <f>IF(N27=3, 750, IF(N27=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M27">
         <f>L27*4</f>
@@ -1320,46 +1338,35 @@
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>https://twitter.com/ReportoCA/status/1301930781745577987?s=20</t>
+          <t>https://www.dailymotion.com/embed/video/x7wyvme</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
-          <t>Entrevista 1</t>
+          <t>Entrevista 6</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>44078</v>
-      </c>
-      <c r="G28" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
+        <v>44127</v>
+      </c>
+      <c r="G28" s="2" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros y Kenia Almengor, gerentes del Área Económica Especial Panamá Pacífico, expresan optimismo ante reapertura el lunes.</t>
+          <t>Entrevista al Ing. Enrique Luna, sobre la inteligencia artificial</t>
         </is>
       </c>
       <c r="K28" t="n">
         <v>20</v>
       </c>
-      <c r="L28">
-        <f>IF(N28=3, 750, IF(N28=1, 1000, ""))</f>
-        <v/>
-      </c>
+      <c r="L28" t="inlineStr"/>
       <c r="M28">
         <f>L28*4</f>
         <v/>
@@ -1374,35 +1381,46 @@
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>https://ecotvpanama.com/programas/eco-news/panama-pacifico-apunta-por-una-robusta-reactivacion-economica_1_65873/#~text=Panam%C3%A1%2014%20de%20septiembre%20del,Panam%C3%A1%20pese%20a%20la%20pandemia.</t>
+          <t>No RADIO PANAMÁ</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>Entrevista 2</t>
+          <t>Mención de Marca 1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Entrevista a César Contreras y Enar Jiménez, voceros de PPG, sobre como Panamá Pacifico apunta por una robusta reactivación económica</t>
+          <t>La tecnología que ayuda a monitorear temperaturas corporales anormales</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>44088</v>
-      </c>
-      <c r="G29" s="2" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+        <v>44106</v>
+      </c>
+      <c r="G29" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Entrevista a César Contreras y Enar Jiménez, voceros de PPG, sobre como Panamá Pacifico apunta por una robusta reactivación económica</t>
+          <t>La tecnología que ayuda a monitorear temperaturas corporales anormales</t>
         </is>
       </c>
       <c r="K29" t="n">
         <v>21</v>
       </c>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29">
+        <f>IF(N29=3, 750, IF(N29=1, 1000, ""))</f>
+        <v/>
+      </c>
       <c r="M29">
         <f>L29*4</f>
         <v/>
@@ -1417,35 +1435,46 @@
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>No ECOTV</t>
+          <t>https://riducaonline.com/2020/10/02/la-tecnologia-que-ayuda-a-monitorear-temperaturas-corporales-anormales/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>Entrevista 2</t>
+          <t>Mención de Marca 2</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Entrevista a César Contreras y Enar Jiménez, voceros de PPG, sobre como Panamá Pacifico apunta por una robusta reactivación económica</t>
+          <t>Conozca cómo la IA cambió la forma de viajar</t>
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>44088</v>
-      </c>
-      <c r="G30" s="2" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
+        <v>44105</v>
+      </c>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Entrevista a César Contreras y Enar Jiménez, voceros de PPG, sobre como Panamá Pacifico apunta por una robusta reactivación económica</t>
+          <t>Conozca cómo la IA cambió la forma de viajar</t>
         </is>
       </c>
       <c r="K30" t="n">
         <v>22</v>
       </c>
-      <c r="L30" t="inlineStr"/>
+      <c r="L30">
+        <f>IF(N30=3, 750, IF(N30=1, 1000, ""))</f>
+        <v/>
+      </c>
       <c r="M30">
         <f>L30*4</f>
         <v/>
@@ -1460,45 +1489,44 @@
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>No NEXTV</t>
+          <t>https://elcapitalfinanciero.com/conozca-como-la-ia-cambio-la-forma-de-viajar/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>Entrevista 3</t>
+          <t>Mención de Marca 2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros, Gerente de Desarrollo estratégico sobre reapertura</t>
+          <t>Conozca cómo la IA cambió la forma de viajar</t>
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>44078</v>
+        <v>44105</v>
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros, Gerente de Desarrollo estratégico sobre reapertura</t>
+          <t>Conozca cómo la IA cambió la forma de viajar</t>
         </is>
       </c>
       <c r="K31" t="n">
         <v>23</v>
       </c>
-      <c r="L31">
-        <f>IF(N31=3, 750, IF(N31=1, 1000, ""))</f>
-        <v/>
+      <c r="L31" t="n">
+        <v>500</v>
       </c>
       <c r="M31">
         <f>L31*4</f>
@@ -1514,35 +1542,46 @@
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=aXvygpKpSwQ</t>
+          <t>https://twitter.com/ElCFPanama/status/1311699596868030465?s=20</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>Entrevista 3</t>
+          <t>Mención de Marca 3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros, Gerente de Desarrollo estratégico sobre reapertura</t>
+          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>44078</v>
-      </c>
-      <c r="G32" s="2" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
+        <v>44134</v>
+      </c>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Entrevista a Hernán Riveros, Gerente de Desarrollo estratégico sobre reapertura</t>
+          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
         </is>
       </c>
       <c r="K32" t="n">
         <v>24</v>
       </c>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32">
+        <f>IF(N32=3, 750, IF(N32=1, 1000, ""))</f>
+        <v/>
+      </c>
       <c r="M32">
         <f>L32*4</f>
         <v/>
@@ -1557,182 +1596,8 @@
       </c>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>No NEXTV</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Entrevista 4</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Entrevista a Stephanie Fleming, Administradora de Trail sobre la educación en tiempos de pandemia</t>
-        </is>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>44091</v>
-      </c>
-      <c r="G33" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Entrevista a Stephanie Fleming, Administradora de Trail sobre la educación en tiempos de pandemia</t>
-        </is>
-      </c>
-      <c r="K33" t="n">
-        <v>25</v>
-      </c>
-      <c r="L33">
-        <f>IF(N33=3, 750, IF(N33=1, 1000, ""))</f>
-        <v/>
-      </c>
-      <c r="M33">
-        <f>L33*4</f>
-        <v/>
-      </c>
-      <c r="O33">
-        <f>IF(N33=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q33">
-        <f>IF(N33=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA33" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=33BjaqncjmQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Entrevista 4</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Entrevista a Stephanie Fleming, Administradora de Trail sobre la educación en tiempos de pandemia</t>
-        </is>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>44091</v>
-      </c>
-      <c r="G34" s="2" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Entrevista a Stephanie Fleming, Administradora de Trail sobre la educación en tiempos de pandemia</t>
-        </is>
-      </c>
-      <c r="K34" t="n">
-        <v>26</v>
-      </c>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34">
-        <f>L34*4</f>
-        <v/>
-      </c>
-      <c r="O34">
-        <f>IF(N34=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q34">
-        <f>IF(N34=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>No NEXTV</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Entrevista 5</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Entrevista a Kemmy Almengor, Gerente de comunicaciones de Panamá Pacífico sobre reapertura de Panamá Pacífico</t>
-        </is>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>44091</v>
-      </c>
-      <c r="G35" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Entrevista a Kemmy Almengor, Gerente de comunicaciones de Panamá Pacífico sobre reapertura de Panamá Pacífico</t>
-        </is>
-      </c>
-      <c r="K35" t="n">
-        <v>27</v>
-      </c>
-      <c r="L35">
-        <f>IF(N35=3, 750, IF(N35=1, 1000, ""))</f>
-        <v/>
-      </c>
-      <c r="M35">
-        <f>L35*4</f>
-        <v/>
-      </c>
-      <c r="O35">
-        <f>IF(N35=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q35">
-        <f>IF(N35=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=zzwTGJuxY4M</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Entrevista 5</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Entrevista a Kemmy Almengor, Gerente de comunicaciones de Panamá Pacífico sobre reapertura de Panamá Pacífico</t>
-        </is>
-      </c>
-      <c r="F36" s="1" t="n">
-        <v>44091</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Entrevista a Kemmy Almengor, Gerente de comunicaciones de Panamá Pacífico sobre reapertura de Panamá Pacífico</t>
-        </is>
-      </c>
-      <c r="K36" t="n">
-        <v>28</v>
+          <t>https://somosimpactopositivo.com/impactando-en-positivo/comsmarket-agencia/</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1761,9 +1626,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G30" r:id="rId22"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G31" r:id="rId23"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G32" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G33" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G34" r:id="rId26"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G35" r:id="rId27"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
New try with heroku - updated Report-Generator.py
</commit_message>
<xml_diff>
--- a/Excel Terminado.xlsx
+++ b/Excel Terminado.xlsx
@@ -330,7 +330,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="D9:AA37"/>
+  <dimension ref="D9:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -341,16 +341,16 @@
     <row r="9">
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mención de Marca 1</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>44105</v>
+        <v>44110</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
@@ -365,7 +365,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
+          <t>Plataforma virtual, clave para ferias inmobiliarias en tiempos de covid-19</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -389,36 +389,46 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>https://somosimpactopositivo.com/impactando-en-positivo/comsmarket-agencia/</t>
+          <t>https://www.laestrella.com.pa/economia/201006/plataforma-virtual-clave-ferias-inmobiliarias-tiempos-covid-19</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mención de Marca 2</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Panamá debe apostar a servicios digitales</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>44105</v>
-      </c>
-      <c r="G10" s="2" t="inlineStr"/>
+        <v>44110</v>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Panamá debe apostar a servicios digitales</t>
+          <t>Plataforma virtual, clave para ferias inmobiliarias en tiempos de covid-19</t>
         </is>
       </c>
       <c r="K10" t="n">
         <v>2</v>
       </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>500</v>
+      </c>
       <c r="M10">
         <f>L10*4</f>
         <v/>
@@ -433,46 +443,45 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>No PANAMÁ AMÉRICA</t>
+          <t>https://twitter.com/ReportoCA/status/1313549638864117760?s=20</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mención de Marca 2</t>
+          <t>Nota de Prensa 1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Panamá debe apostar a servicios digitales</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>44105</v>
+        <v>44110</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Panamá debe apostar a servicios digitales</t>
+          <t>Plataforma virtual, clave para ferias inmobiliarias en tiempos de covid-19</t>
         </is>
       </c>
       <c r="K11" t="n">
         <v>3</v>
       </c>
-      <c r="L11">
-        <f>IF(N11=3, 750, IF(N11=1, 1000, ""))</f>
-        <v/>
+      <c r="L11" t="n">
+        <v>500</v>
       </c>
       <c r="M11">
         <f>L11*4</f>
@@ -488,7 +497,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>https://www.pressreader.com/panama/panama-america/20201001/282020444744622</t>
+          <t>https://twitter.com/EstrellaOnline/status/1313554875150721024?s=20</t>
         </is>
       </c>
     </row>
@@ -500,11 +509,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>44105</v>
+        <v>44111</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
@@ -519,7 +528,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Panamá ante el reto de ser una economía desarrollada</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="K12" t="n">
@@ -543,7 +552,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>https://www.prensa.com/impresa/economia/panama-ante-el-reto-de-ser-una-economia-desarrollada/</t>
+          <t>https://elcapitalfinanciero.com/modalidad-virtual-impacta-a-las-principales-ferias-comerciales-de-la-region/</t>
         </is>
       </c>
     </row>
@@ -555,11 +564,11 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>44105</v>
+        <v>44111</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
@@ -574,7 +583,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="K13" t="n">
@@ -598,7 +607,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>https://www.panama24horas.com.pa/panama/economia-competitividad-y-futuro-de-panam/</t>
+          <t>http://www.findglocal.com/PA/Panama-City/22056981168/El-Espectador-de-Panam%C3%A1</t>
         </is>
       </c>
     </row>
@@ -610,11 +619,11 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>44105</v>
+        <v>44111</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
@@ -629,7 +638,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="K14" t="n">
@@ -652,7 +661,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>https://twitter.com/sabribacal/status/1311626659720765441?s=20</t>
+          <t>https://twitter.com/ElCFPanama/status/1313866365854461953?s=20</t>
         </is>
       </c>
     </row>
@@ -664,15 +673,15 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>44105</v>
+        <v>44111</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -683,7 +692,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="K15" t="n">
@@ -706,7 +715,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>https://twitter.com/Panama24horas/status/1311536585993785346?s=20</t>
+          <t>https://www.instagram.com/p/CGECFkHnvmw/?igshid=a9bowmzakvt8</t>
         </is>
       </c>
     </row>
@@ -718,34 +727,33 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>44118</v>
+        <v>44111</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="K16" t="n">
         <v>8</v>
       </c>
-      <c r="L16">
-        <f>IF(N16=3, 750, IF(N16=1, 1000, ""))</f>
-        <v/>
+      <c r="L16" t="n">
+        <v>500</v>
       </c>
       <c r="M16">
         <f>L16*4</f>
@@ -761,7 +769,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>https://panamaaldia.news/el-aporte-de-todos-los-sectores-es-clave-para-reactivar-nuestra-economia/</t>
+          <t>https://twitter.com/EstrellaOnline/status/1313773683941478401?s=20</t>
         </is>
       </c>
     </row>
@@ -773,34 +781,33 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>44118</v>
+        <v>44111</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
         </is>
       </c>
       <c r="K17" t="n">
         <v>9</v>
       </c>
-      <c r="L17">
-        <f>IF(N17=3, 750, IF(N17=1, 1000, ""))</f>
-        <v/>
+      <c r="L17" t="n">
+        <v>500</v>
       </c>
       <c r="M17">
         <f>L17*4</f>
@@ -816,23 +823,23 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>https://verpanama.com/aporte-de-todos-los-sectores-clave-para-reactivacion/</t>
+          <t>https://www.facebook.com/LaEstrelladePanama/photos/capac-plataforma-virtual-clave-para-ferias-inmobiliarias-en-tiempos-de-covid-19-/3362490347121567/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
         <is>
-          <t>Nota de Prensa 1</t>
+          <t>Nota de Prensa 2</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>44118</v>
+        <v>44117</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
@@ -847,7 +854,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="K18" t="n">
@@ -871,45 +878,46 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>https://www.panama24horas.com.pa/panama/el-aporte-de-todos-los-sectores-es-clave-para-reactivar-nuestra-economia/</t>
+          <t>https://www.panama24horas.com.pa/centroamerica/encuentra24-cumple-15-anos-siendo-la-plataforma-lider-en-la-region/#~text=existencia%20de%20Encuentra24.-,Este%20mes%2C%20la%20plataforma%20digital%20l%C3%ADder%20en%20la%20regi%C3%B3n%2C%20celebra,nuestra%20regi%C3%B3n%20y%20el%20Caribe.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
         <is>
-          <t>Nota de Prensa 1</t>
+          <t>Nota de Prensa 2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Economía, Competitividad y futuro de Panamá / El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>44118</v>
+        <v>44117</v>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>El aporte de todos los sectores es clave para reactivar nuestra economía</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="K19" t="n">
         <v>11</v>
       </c>
-      <c r="L19" t="n">
-        <v>500</v>
+      <c r="L19">
+        <f>IF(N19=3, 750, IF(N19=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M19">
         <f>L19*4</f>
@@ -925,23 +933,23 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>https://twitter.com/verpanama1/status/1316529160010051584?s=20</t>
+          <t>https://panamaaldia.news/encuentra24-cumple-15-anos-siendo-la-plataforma-lider-en-la-region/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mención de Marca 3</t>
+          <t>Nota de Prensa 2</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>En la conferencia virtual de Café con La Prensa, René Quevedo, analista y consultor laboral; y Adriana Angarita, rectora de la Universidad del Istmo y presidenta de la Asociación de Universidades Privadas de Panamá analizaron la realidad de la situación laboral panameña.</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>44118</v>
+        <v>44119</v>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
@@ -956,7 +964,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>En la conferencia virtual de Café con La Prensa, René Quevedo, analista y consultor laboral; y Adriana Angarita, rectora de la Universidad del Istmo y presidenta de la Asociación de Universidades Privadas de Panamá analizaron la realidad de la situación laboral panameña.</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="K20" t="n">
@@ -980,45 +988,46 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>https://www.prensa.com/economia/panama-se-enfrenta-a-una-situacion-complicada-en-materia-laboral-producto-de-la-pandemia/</t>
+          <t>http://madridhoy.info/search.php?pagina=19&amp;s=%40%40Panam%C3%A1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
         <is>
-          <t>Mención de Marca 3</t>
+          <t>Nota de Prensa 2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>En la conferencia virtual de Café con La Prensa, René Quevedo, analista y consultor laboral; y Adriana Angarita, rectora de la Universidad del Istmo y presidenta de la Asociación de Universidades Privadas de Panamá analizaron la realidad de la situación laboral panameña.</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>44118</v>
+        <v>44131</v>
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>En la conferencia virtual de Café con La Prensa, René Quevedo, analista y consultor laboral; y Adriana Angarita, rectora de la Universidad del Istmo y presidenta de la Asociación de Universidades Privadas de Panamá analizaron la realidad de la situación laboral panameña.</t>
+          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
         </is>
       </c>
       <c r="K21" t="n">
         <v>13</v>
       </c>
-      <c r="L21" t="n">
-        <v>500</v>
+      <c r="L21">
+        <f>IF(N21=3, 750, IF(N21=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M21">
         <f>L21*4</f>
@@ -1034,45 +1043,46 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>https://twitter.com/prensacom/status/1316391133677789187?s=20</t>
+          <t>https://somosimpactopositivo.com/impacto-economico/aniversario-encuentra24/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="D22" t="inlineStr">
         <is>
-          <t>Mención de Marca 3</t>
+          <t>Nota de Prensa 3 (Septiembre)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>En la conferencia virtual de Café con La Prensa, René Quevedo, analista y consultor laboral; y Adriana Angarita, rectora de la Universidad del Istmo y presidenta de la Asociación de Universidades Privadas de Panamá analizaron la realidad de la situación laboral panameña.</t>
+          <t>Panamá en la mira de compradores internacionales de bienes raíces</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>44118</v>
+        <v>44106</v>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>En la conferencia virtual de Café con La Prensa, René Quevedo, analista y consultor laboral; y Adriana Angarita, rectora de la Universidad del Istmo y presidenta de la Asociación de Universidades Privadas de Panamá analizaron la realidad de la situación laboral panameña.</t>
+          <t>Panamá en la mira de compradores internacionales de bienes raíces</t>
         </is>
       </c>
       <c r="K22" t="n">
         <v>14</v>
       </c>
-      <c r="L22" t="n">
-        <v>500</v>
+      <c r="L22">
+        <f>IF(N22=3, 750, IF(N22=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M22">
         <f>L22*4</f>
@@ -1088,23 +1098,23 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>https://twitter.com/prensacom/status/1316387283554258952?s=20</t>
+          <t>https://panamaaldia.news/panama-en-la-mira-de-compradores-internacionales-de-bienes-raices-2/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>Mención de Marca 4</t>
+          <t>Mención de Marca 1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Hay una serie de actividades económicas más perjudicadas que otras por la pandemia. Adriana Angarita, presidenta de la Asociación de Universidades Privadas de Panamá (Auppa), dijo que en términos generales los sectores que pierden relevancia son la construcción, la aviación, el turismo y los servicios financieros.</t>
+          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>44119</v>
+        <v>44109</v>
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
@@ -1119,7 +1129,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Hay una serie de actividades económicas más perjudicadas que otras por la pandemia. Adriana Angarita, presidenta de la Asociación de Universidades Privadas de Panamá (Auppa), dijo que en términos generales los sectores que pierden relevancia son la construcción, la aviación, el turismo y los servicios financieros.</t>
+          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
         </is>
       </c>
       <c r="K23" t="n">
@@ -1143,23 +1153,23 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>https://www.prensa.com/impresa/economia/incertidumbre-principal-obstaculo-en-la-recuperacion/</t>
+          <t>https://www.critica.com.pa/nacional/el-consumo-siempre-vuelve-589324</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="D24" t="inlineStr">
         <is>
-          <t>Mención de Marca 4</t>
+          <t>Mención de Marca 1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Hay una serie de actividades económicas más perjudicadas que otras por la pandemia. Adriana Angarita, presidenta de la Asociación de Universidades Privadas de Panamá (Auppa), dijo que en términos generales los sectores que pierden relevancia son la construcción, la aviación, el turismo y los servicios financieros.</t>
+          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>44119</v>
+        <v>44109</v>
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
@@ -1174,7 +1184,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Hay una serie de actividades económicas más perjudicadas que otras por la pandemia. Adriana Angarita, presidenta de la Asociación de Universidades Privadas de Panamá (Auppa), dijo que en términos generales los sectores que pierden relevancia son la construcción, la aviación, el turismo y los servicios financieros.</t>
+          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
         </is>
       </c>
       <c r="K24" t="n">
@@ -1197,45 +1207,46 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>https://twitter.com/prensacom/status/1316768997329821699?s=20</t>
+          <t>https://twitter.com/criticaenlinea/status/1313004115430178817?s=20</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="D25" t="inlineStr">
         <is>
-          <t>Mención de Marca 4</t>
+          <t>Nota de Prensa 4 (Septiembre)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Hay una serie de actividades económicas más perjudicadas que otras por la pandemia. Adriana Angarita, presidenta de la Asociación de Universidades Privadas de Panamá (Auppa), dijo que en términos generales los sectores que pierden relevancia son la construcción, la aviación, el turismo y los servicios financieros.</t>
+          <t>Vivir en espacios abiertos, es la alternativa que prefieren los usuarios de plataformas digitales luego de la pandemia</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>44119</v>
+        <v>44114</v>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Hay una serie de actividades económicas más perjudicadas que otras por la pandemia. Adriana Angarita, presidenta de la Asociación de Universidades Privadas de Panamá (Auppa), dijo que en términos generales los sectores que pierden relevancia son la construcción, la aviación, el turismo y los servicios financieros.</t>
+          <t>Vivir en espacios abiertos, alternativa de usuarios de plataformas digitales</t>
         </is>
       </c>
       <c r="K25" t="n">
         <v>17</v>
       </c>
-      <c r="L25" t="n">
-        <v>500</v>
+      <c r="L25">
+        <f>IF(N25=3, 750, IF(N25=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M25">
         <f>L25*4</f>
@@ -1251,47 +1262,36 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>https://twitter.com/prensacom/status/1316768686934495233?s=20</t>
+          <t>https://www.periodicoequilibrium.com/vivir-en-espacios-abiertos-alternativa-de-usuarios-de-plataformas-digitales/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="D26" t="inlineStr">
         <is>
-          <t>Nota de Prensa 2</t>
+          <t>Entrevista 1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>44118</v>
-      </c>
-      <c r="G26" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
+        <v>44133</v>
+      </c>
+      <c r="G26" s="2" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
         </is>
       </c>
       <c r="K26" t="n">
         <v>18</v>
       </c>
-      <c r="L26">
-        <f>IF(N26=3, 750, IF(N26=1, 1000, ""))</f>
-        <v/>
-      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26">
         <f>L26*4</f>
         <v/>
@@ -1306,23 +1306,23 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>https://panamaaldia.news/futuro-de-panama-a-traves-del-talento-humano-una-mirada-desde-el-liderazgo-juvenil/</t>
+          <t>No Metrolibre</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="D27" t="inlineStr">
         <is>
-          <t>Nota de Prensa 2</t>
+          <t>Entrevista 1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>44191</v>
+        <v>44133</v>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
         </is>
       </c>
       <c r="K27" t="n">
@@ -1361,46 +1361,45 @@
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>https://riducaonline.com/2020/10/26/futuro-de-panama-a-traves-del-talento-humano-una-mirada-desde-el-liderazgo-juvenil/</t>
+          <t>https://www.metrolibre.com/econom%C3%ADa/185546-comercio-electr%C3%B3nico-crece-en-un-150-por-la-pandemia.html</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
-          <t>Nota de Prensa 2</t>
+          <t>Entrevista 1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>44131</v>
+        <v>44133</v>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
         </is>
       </c>
       <c r="K28" t="n">
         <v>20</v>
       </c>
-      <c r="L28">
-        <f>IF(N28=3, 750, IF(N28=1, 1000, ""))</f>
-        <v/>
+      <c r="L28" t="n">
+        <v>500</v>
       </c>
       <c r="M28">
         <f>L28*4</f>
@@ -1416,45 +1415,46 @@
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>https://www.metrolibre.com/nacionales/185408-j%C3%B3venes-l%C3%ADderes-compartir%C3%A1n-su-visi%C3%B3n-del-futuro-de-panam%C3%A1.html</t>
+          <t>https://twitter.com/MetroLibrePTY/status/1321754944316207105?s=20</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>Nota de Prensa 2</t>
+          <t>Mención de Marca 2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>44131</v>
+        <v>44134</v>
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
+          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
         </is>
       </c>
       <c r="K29" t="n">
         <v>21</v>
       </c>
-      <c r="L29" t="n">
-        <v>500</v>
+      <c r="L29">
+        <f>IF(N29=3, 750, IF(N29=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M29">
         <f>L29*4</f>
@@ -1470,423 +1470,7 @@
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>https://twitter.com/MetroLibrePTY/status/1321191696344907777?s=20</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 2</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
-        </is>
-      </c>
-      <c r="F30" s="1" t="n">
-        <v>44132</v>
-      </c>
-      <c r="G30" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
-        </is>
-      </c>
-      <c r="K30" t="n">
-        <v>22</v>
-      </c>
-      <c r="L30">
-        <f>IF(N30=3, 750, IF(N30=1, 1000, ""))</f>
-        <v/>
-      </c>
-      <c r="M30">
-        <f>L30*4</f>
-        <v/>
-      </c>
-      <c r="O30">
-        <f>IF(N30=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q30">
-        <f>IF(N30=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>https://www.panama24horas.com.pa/comunidad/futuro-de-panama-a-traves-del-talento-humano-una-mirada-desde-el-liderazgo-juvenil/</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 2</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
-        </is>
-      </c>
-      <c r="F31" s="1" t="n">
-        <v>44132</v>
-      </c>
-      <c r="G31" s="2" t="inlineStr">
-        <is>
-          <t>Twitter</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>1 post</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
-        </is>
-      </c>
-      <c r="K31" t="n">
-        <v>23</v>
-      </c>
-      <c r="L31" t="n">
-        <v>500</v>
-      </c>
-      <c r="M31">
-        <f>L31*4</f>
-        <v/>
-      </c>
-      <c r="O31">
-        <f>IF(N31=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q31">
-        <f>IF(N31=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>https://twitter.com/Panama24horas/status/1321514330391674880?s=20</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 2</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
-        </is>
-      </c>
-      <c r="F32" s="1" t="n">
-        <v>44132</v>
-      </c>
-      <c r="G32" s="2" t="inlineStr">
-        <is>
-          <t>Instagram</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>1 post</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Futuro de Panamá a través del talento humano una mirada desde el liderazgo juvenil</t>
-        </is>
-      </c>
-      <c r="K32" t="n">
-        <v>24</v>
-      </c>
-      <c r="L32" t="n">
-        <v>500</v>
-      </c>
-      <c r="M32">
-        <f>L32*4</f>
-        <v/>
-      </c>
-      <c r="O32">
-        <f>IF(N32=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q32">
-        <f>IF(N32=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/p/CG5ZABMBLht/?igshid=sc2z73zp4xva</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Entrevista 1</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>44126</v>
-      </c>
-      <c r="G33" s="2" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="K33" t="n">
-        <v>25</v>
-      </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33">
-        <f>L33*4</f>
-        <v/>
-      </c>
-      <c r="O33">
-        <f>IF(N33=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q33">
-        <f>IF(N33=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA33" t="inlineStr">
-        <is>
-          <t>No NEXTV 345</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Entrevista 1</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>44126</v>
-      </c>
-      <c r="G34" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="K34" t="n">
-        <v>26</v>
-      </c>
-      <c r="L34">
-        <f>IF(N34=3, 750, IF(N34=1, 1000, ""))</f>
-        <v/>
-      </c>
-      <c r="M34">
-        <f>L34*4</f>
-        <v/>
-      </c>
-      <c r="O34">
-        <f>IF(N34=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q34">
-        <f>IF(N34=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=_mPWJjJlK1I</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Entrevista 1</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>44126</v>
-      </c>
-      <c r="G35" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="K35" t="n">
-        <v>27</v>
-      </c>
-      <c r="L35">
-        <f>IF(N35=3, 750, IF(N35=1, 1000, ""))</f>
-        <v/>
-      </c>
-      <c r="M35">
-        <f>L35*4</f>
-        <v/>
-      </c>
-      <c r="O35">
-        <f>IF(N35=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q35">
-        <f>IF(N35=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>https://nexnoticias.ruplayers.com/xZ-Hu67Nfpx_aX0/entrevista-a-adriana-angarita-presidente-de-la-asoc-auppa.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Entrevista 1</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="F36" s="1" t="n">
-        <v>44126</v>
-      </c>
-      <c r="G36" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="K36" t="n">
-        <v>28</v>
-      </c>
-      <c r="L36">
-        <f>IF(N36=3, 750, IF(N36=1, 1000, ""))</f>
-        <v/>
-      </c>
-      <c r="M36">
-        <f>L36*4</f>
-        <v/>
-      </c>
-      <c r="O36">
-        <f>IF(N36=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q36">
-        <f>IF(N36=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA36" t="inlineStr">
-        <is>
-          <t>https://pa.domiplay.net/video/entrevista-a-adriana-angarita-presidente-22-10-20-nex-mpk1i</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Entrevista 2</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="F37" s="1" t="n">
-        <v>44127</v>
-      </c>
-      <c r="G37" s="2" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Entrevista a Adriana Angarita sobre el Futuro de Panamá a través del talento humano</t>
-        </is>
-      </c>
-      <c r="K37" t="n">
-        <v>29</v>
-      </c>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37">
-        <f>L37*4</f>
-        <v/>
-      </c>
-      <c r="O37">
-        <f>IF(N37=1,1,"")</f>
-        <v/>
-      </c>
-      <c r="Q37">
-        <f>IF(N37=3,1,"")</f>
-        <v/>
-      </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>No Radio Panamá 1200</t>
+          <t>https://somosimpactopositivo.com/impactando-en-positivo/comsmarket-agencia/</t>
         </is>
       </c>
     </row>
@@ -1913,14 +1497,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G27" r:id="rId19"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G28" r:id="rId20"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G29" r:id="rId21"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G30" r:id="rId22"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G31" r:id="rId23"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G32" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G33" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G34" r:id="rId26"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G35" r:id="rId27"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G36" r:id="rId28"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G37" r:id="rId29"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Troubleshooting for word document and index list issues.
</commit_message>
<xml_diff>
--- a/Excel Terminado.xlsx
+++ b/Excel Terminado.xlsx
@@ -330,7 +330,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="D9:AA29"/>
+  <dimension ref="F9:AA56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -339,18 +339,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="9">
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F9" s="1" t="n">
-        <v>44110</v>
+        <v>44117</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
@@ -365,7 +355,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Plataforma virtual, clave para ferias inmobiliarias en tiempos de covid-19</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -389,45 +379,36 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>https://www.laestrella.com.pa/economia/201006/plataforma-virtual-clave-ferias-inmobiliarias-tiempos-covid-19</t>
+          <t>https://www.panama24horas.com.pa/empresas/expo-feria-de-la-asociacion-de-empresas-del-area-panama-pacifico-un-encuentro-de-crecimiento-bienestar-y-emprendimiento/</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F10" s="1" t="n">
-        <v>44110</v>
+        <v>44117</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Plataforma virtual, clave para ferias inmobiliarias en tiempos de covid-19</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K10" t="n">
         <v>2</v>
       </c>
-      <c r="L10" t="n">
-        <v>500</v>
+      <c r="L10">
+        <f>IF(N10=3, 750, IF(N10=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M10">
         <f>L10*4</f>
@@ -443,45 +424,36 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>https://twitter.com/ReportoCA/status/1313549638864117760?s=20</t>
+          <t>https://panamaaldia.news/expo-feria-de-la-asociacion-de-empresas-del-area-panama-pacifico-un-encuentro-de-crecimiento-bienestar-y-emprendimiento/</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F11" s="1" t="n">
-        <v>44110</v>
+        <v>44118</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Plataforma virtual, clave para ferias inmobiliarias en tiempos de covid-19</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K11" t="n">
         <v>3</v>
       </c>
-      <c r="L11" t="n">
-        <v>500</v>
+      <c r="L11">
+        <f>IF(N11=3, 750, IF(N11=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M11">
         <f>L11*4</f>
@@ -497,23 +469,13 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>https://twitter.com/EstrellaOnline/status/1313554875150721024?s=20</t>
+          <t>https://panamaaldia.news/expo-feria-de-la-asociacion-de-empresas-del-area-panama-pacifico-un-encuentro-de-crecimiento-bienestar-y-emprendimiento-2/</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F12" s="1" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
@@ -528,7 +490,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K12" t="n">
@@ -552,46 +514,35 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>https://elcapitalfinanciero.com/modalidad-virtual-impacta-a-las-principales-ferias-comerciales-de-la-region/</t>
+          <t>https://elcapitalfinanciero.com/empresa-de-panama-pacifico-preparan-una-nueva-version-de-su-feria-comercial/</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F13" s="1" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K13" t="n">
         <v>5</v>
       </c>
-      <c r="L13">
-        <f>IF(N13=3, 750, IF(N13=1, 1000, ""))</f>
-        <v/>
+      <c r="L13" t="n">
+        <v>500</v>
       </c>
       <c r="M13">
         <f>L13*4</f>
@@ -607,45 +558,36 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>http://www.findglocal.com/PA/Panama-City/22056981168/El-Espectador-de-Panam%C3%A1</t>
+          <t>https://twitter.com/ElCFPanama/status/1316409889393123330?s=20</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F14" s="1" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K14" t="n">
         <v>6</v>
       </c>
-      <c r="L14" t="n">
-        <v>500</v>
+      <c r="L14">
+        <f>IF(N14=3, 750, IF(N14=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M14">
         <f>L14*4</f>
@@ -661,45 +603,36 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>https://twitter.com/ElCFPanama/status/1313866365854461953?s=20</t>
+          <t>http://prnoticiaspanama.com/expo-feria-de-la-asociacion-de-empresas-del-area-panama-pacifico-un-encuentro-de-crecimiento-bienestar-y-emprendimiento/</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F15" s="1" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K15" t="n">
         <v>7</v>
       </c>
-      <c r="L15" t="n">
-        <v>500</v>
+      <c r="L15">
+        <f>IF(N15=3, 750, IF(N15=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M15">
         <f>L15*4</f>
@@ -715,45 +648,36 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/CGECFkHnvmw/?igshid=a9bowmzakvt8</t>
+          <t>https://verpanama.com/expo-feria-2020-area-panama-pacifico/</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F16" s="1" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K16" t="n">
         <v>8</v>
       </c>
-      <c r="L16" t="n">
-        <v>500</v>
+      <c r="L16">
+        <f>IF(N16=3, 750, IF(N16=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M16">
         <f>L16*4</f>
@@ -769,45 +693,36 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>https://twitter.com/EstrellaOnline/status/1313773683941478401?s=20</t>
+          <t>https://xpectativapty.com/2020/10/14/expo-feria-de-la-asociacion-de-empresas-del-area-panama-pacifico-un-encuentro-de-crecimiento-bienestar-y-emprendimiento/</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 1</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
-        </is>
-      </c>
       <c r="F17" s="1" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Modalidad virtual impacta a las principales ferias comerciales de la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K17" t="n">
         <v>9</v>
       </c>
-      <c r="L17" t="n">
-        <v>500</v>
+      <c r="L17">
+        <f>IF(N17=3, 750, IF(N17=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M17">
         <f>L17*4</f>
@@ -823,23 +738,13 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/LaEstrelladePanama/photos/capac-plataforma-virtual-clave-para-ferias-inmobiliarias-en-tiempos-de-covid-19-/3362490347121567/</t>
+          <t>https://www.eventos507.com/expo-feria-2020-de-panama-pacifico/</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 2</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
-        </is>
-      </c>
       <c r="F18" s="1" t="n">
-        <v>44117</v>
+        <v>44119</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
@@ -854,7 +759,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K18" t="n">
@@ -878,46 +783,35 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>https://www.panama24horas.com.pa/centroamerica/encuentra24-cumple-15-anos-siendo-la-plataforma-lider-en-la-region/#~text=existencia%20de%20Encuentra24.-,Este%20mes%2C%20la%20plataforma%20digital%20l%C3%ADder%20en%20la%20regi%C3%B3n%2C%20celebra,nuestra%20regi%C3%B3n%20y%20el%20Caribe.</t>
+          <t>https://profesionalespanama.net/nacionales/anuncian-feria-de-la-asociacion-de-empresas-del-area-panama-pacifico/</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 2</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
-        </is>
-      </c>
       <c r="F19" s="1" t="n">
-        <v>44117</v>
+        <v>44119</v>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K19" t="n">
         <v>11</v>
       </c>
-      <c r="L19">
-        <f>IF(N19=3, 750, IF(N19=1, 1000, ""))</f>
-        <v/>
+      <c r="L19" t="n">
+        <v>500</v>
       </c>
       <c r="M19">
         <f>L19*4</f>
@@ -933,21 +827,11 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>https://panamaaldia.news/encuentra24-cumple-15-anos-siendo-la-plataforma-lider-en-la-region/</t>
+          <t>https://twitter.com/NoticieroPanama/status/1316776613120540677?s=20</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 2</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
-        </is>
-      </c>
       <c r="F20" s="1" t="n">
         <v>44119</v>
       </c>
@@ -964,7 +848,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K20" t="n">
@@ -988,47 +872,26 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>http://madridhoy.info/search.php?pagina=19&amp;s=%40%40Panam%C3%A1</t>
+          <t>https://www.panamaamerica.com.pa/economia/anuncian-feria-asociacion-empresas-del-area-panama-pacifico-117409</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 2</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
-        </is>
-      </c>
       <c r="F21" s="1" t="n">
-        <v>44131</v>
-      </c>
-      <c r="G21" s="2" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
+        <v>44120</v>
+      </c>
+      <c r="G21" s="2" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>1 página</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Encuentra24 cumple 15 años siendo la plataforma líder en la región</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K21" t="n">
         <v>13</v>
       </c>
-      <c r="L21">
-        <f>IF(N21=3, 750, IF(N21=1, 1000, ""))</f>
-        <v/>
-      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21">
         <f>L21*4</f>
         <v/>
@@ -1043,23 +906,13 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>https://somosimpactopositivo.com/impacto-economico/aniversario-encuentra24/</t>
+          <t>No  Panamá América</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 3 (Septiembre)</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Panamá en la mira de compradores internacionales de bienes raíces</t>
-        </is>
-      </c>
       <c r="F22" s="1" t="n">
-        <v>44106</v>
+        <v>44120</v>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
@@ -1074,7 +927,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Panamá en la mira de compradores internacionales de bienes raíces</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K22" t="n">
@@ -1098,23 +951,13 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>https://panamaaldia.news/panama-en-la-mira-de-compradores-internacionales-de-bienes-raices-2/</t>
+          <t>https://grupostt.com/2020/10/16/expo-feria-de-empresas-panama-pacifico-2020/</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Mención de Marca 1</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
-        </is>
-      </c>
       <c r="F23" s="1" t="n">
-        <v>44109</v>
+        <v>44120</v>
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
@@ -1129,7 +972,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K23" t="n">
@@ -1153,45 +996,36 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>https://www.critica.com.pa/nacional/el-consumo-siempre-vuelve-589324</t>
+          <t>https://www.pressreader.com/panama/panama-america/20201016/281745566866116</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Mención de Marca 1</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
-        </is>
-      </c>
       <c r="F24" s="1" t="n">
-        <v>44109</v>
+        <v>44123</v>
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
-          <t>1 post</t>
+          <t>1 página</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>También mencionó el consumo del comercio electrónico, a través de sitios como por ejemplo Encuentra24 que siempre ha sido de los sitios más visitados de Panamá, Amazon, AliExpress que viene siendo la versión más comercial de Alibaba.</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K24" t="n">
         <v>16</v>
       </c>
-      <c r="L24" t="n">
-        <v>500</v>
+      <c r="L24">
+        <f>IF(N24=3, 750, IF(N24=1, 1000, ""))</f>
+        <v/>
       </c>
       <c r="M24">
         <f>L24*4</f>
@@ -1207,46 +1041,35 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>https://twitter.com/criticaenlinea/status/1313004115430178817?s=20</t>
+          <t>https://www.viajesboletin.com/categorias/principales/panama/76501-anuncian-feria-de-la-asociacion-de-empresas-del-area-panama-pacifico/</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Nota de Prensa 4 (Septiembre)</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Vivir en espacios abiertos, es la alternativa que prefieren los usuarios de plataformas digitales luego de la pandemia</t>
-        </is>
-      </c>
       <c r="F25" s="1" t="n">
-        <v>44114</v>
+        <v>44124</v>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Vivir en espacios abiertos, alternativa de usuarios de plataformas digitales</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K25" t="n">
         <v>17</v>
       </c>
-      <c r="L25">
-        <f>IF(N25=3, 750, IF(N25=1, 1000, ""))</f>
-        <v/>
+      <c r="L25" t="n">
+        <v>500</v>
       </c>
       <c r="M25">
         <f>L25*4</f>
@@ -1262,36 +1085,36 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>https://www.periodicoequilibrium.com/vivir-en-espacios-abiertos-alternativa-de-usuarios-de-plataformas-digitales/</t>
+          <t>https://twitter.com/BoletinViajes/status/1318537453922258944?s=20</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Entrevista 1</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
-        </is>
-      </c>
       <c r="F26" s="1" t="n">
-        <v>44133</v>
-      </c>
-      <c r="G26" s="2" t="inlineStr"/>
+        <v>44124</v>
+      </c>
+      <c r="G26" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K26" t="n">
         <v>18</v>
       </c>
-      <c r="L26" t="inlineStr"/>
+      <c r="L26" t="n">
+        <v>500</v>
+      </c>
       <c r="M26">
         <f>L26*4</f>
         <v/>
@@ -1306,23 +1129,13 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>No Metrolibre</t>
+          <t>https://twitter.com/iberoamericav/status/1318552327297564672?s=20</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Entrevista 1</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
-        </is>
-      </c>
       <c r="F27" s="1" t="n">
-        <v>44133</v>
+        <v>44124</v>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
@@ -1337,7 +1150,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K27" t="n">
@@ -1361,23 +1174,13 @@
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>https://www.metrolibre.com/econom%C3%ADa/185546-comercio-electr%C3%B3nico-crece-en-un-150-por-la-pandemia.html</t>
+          <t>https://www.diaadia.com.pa/el-pais/mitradel-participa-de-la-expo-feria-de-panama-pacifico-2020-371552</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Entrevista 1</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
-        </is>
-      </c>
       <c r="F28" s="1" t="n">
-        <v>44133</v>
+        <v>44124</v>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
@@ -1392,7 +1195,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Entrevista a Wendy Jordán sobre Comercio electrónico crece en un 150% por la pandemia</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K28" t="n">
@@ -1415,46 +1218,35 @@
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>https://twitter.com/MetroLibrePTY/status/1321754944316207105?s=20</t>
+          <t>https://twitter.com/DiaaDiaPa/status/1318688449038184448?s=20</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Mención de Marca 2</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
-        </is>
-      </c>
       <c r="F29" s="1" t="n">
-        <v>44134</v>
+        <v>44125</v>
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>1 página</t>
+          <t>1 post</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Entre las experiencias de éxito que Comsmarket ha sumado en este 2020 está el trabajo con Panamá Pacífico, Volkswagen, Encuentra24, Dahua Technology, la Asociación de Universidades Particulares de Panamá, UMECIT y Tambor S.A.</t>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
         </is>
       </c>
       <c r="K29" t="n">
         <v>21</v>
       </c>
-      <c r="L29">
-        <f>IF(N29=3, 750, IF(N29=1, 1000, ""))</f>
-        <v/>
+      <c r="L29" t="n">
+        <v>500</v>
       </c>
       <c r="M29">
         <f>L29*4</f>
@@ -1470,7 +1262,1059 @@
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>https://somosimpactopositivo.com/impactando-en-positivo/comsmarket-agencia/</t>
+          <t>https://twitter.com/DiaaDiaPa/status/1318780301364121601?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="F30" s="1" t="n">
+        <v>44125</v>
+      </c>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>22</v>
+      </c>
+      <c r="L30" t="n">
+        <v>500</v>
+      </c>
+      <c r="M30">
+        <f>L30*4</f>
+        <v/>
+      </c>
+      <c r="O30">
+        <f>IF(N30=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q30">
+        <f>IF(N30=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>https://twitter.com/DiaaDiaPa/status/1319047059463409664?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="F31" s="1" t="n">
+        <v>44125</v>
+      </c>
+      <c r="G31" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>23</v>
+      </c>
+      <c r="L31" t="n">
+        <v>500</v>
+      </c>
+      <c r="M31">
+        <f>L31*4</f>
+        <v/>
+      </c>
+      <c r="O31">
+        <f>IF(N31=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q31">
+        <f>IF(N31=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>https://twitter.com/DiaaDiaPa/status/1319092357459931136?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="F32" s="1" t="n">
+        <v>44125</v>
+      </c>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>24</v>
+      </c>
+      <c r="L32">
+        <f>IF(N32=3, 750, IF(N32=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M32">
+        <f>L32*4</f>
+        <v/>
+      </c>
+      <c r="O32">
+        <f>IF(N32=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q32">
+        <f>IF(N32=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>https://www.panama24horas.com.pa/panama/mitradel-participa-de-la-expo-feria-de-adedapp-2020/</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="F33" s="1" t="n">
+        <v>44126</v>
+      </c>
+      <c r="G33" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Expo Feria de la Asociación de Empresas del Área Panamá Pacífico, un encuentro de crecimiento, bienestar y emprendimiento</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>25</v>
+      </c>
+      <c r="L33" t="n">
+        <v>500</v>
+      </c>
+      <c r="M33">
+        <f>L33*4</f>
+        <v/>
+      </c>
+      <c r="O33">
+        <f>IF(N33=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q33">
+        <f>IF(N33=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t>https://twitter.com/DiaaDiaPa/status/1319454745279582209?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="F34" s="1" t="n">
+        <v>44114</v>
+      </c>
+      <c r="G34" s="2" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Entrevista a Juan Mckay sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>26</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34">
+        <f>L34*4</f>
+        <v/>
+      </c>
+      <c r="O34">
+        <f>IF(N34=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q34">
+        <f>IF(N34=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>No Radio Panamá 265 segundos</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="F35" s="1" t="n">
+        <v>44114</v>
+      </c>
+      <c r="G35" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Inaugura Expo Feria de ADEDAP, se centrará en Turismo, Tecnología, Educación, Emprendimientos y Vacantes</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>27</v>
+      </c>
+      <c r="L35">
+        <f>IF(N35=3, 750, IF(N35=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M35">
+        <f>L35*4</f>
+        <v/>
+      </c>
+      <c r="O35">
+        <f>IF(N35=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q35">
+        <f>IF(N35=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>https://www.radiopanama.com.pa/noticias/actualidad/inaugura-expo-feria-de-adedap-se-centrara-en-turismo-tecnologia-educacion-emprendimientos-y-vacantes/20201020/nota/4079168.aspx</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="F36" s="1" t="n">
+        <v>44124</v>
+      </c>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Inaugura Expo Feria de ADEDAP, se centrará en Turismo, Tecnología, Educación, Emprendimientos y Vacantes</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>28</v>
+      </c>
+      <c r="L36" t="n">
+        <v>500</v>
+      </c>
+      <c r="M36">
+        <f>L36*4</f>
+        <v/>
+      </c>
+      <c r="O36">
+        <f>IF(N36=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q36">
+        <f>IF(N36=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>https://twitter.com/radiopanama/status/1318771493799538688?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="F37" s="1" t="n">
+        <v>44124</v>
+      </c>
+      <c r="G37" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Inaugura Expo Feria de ADEDAP, se centrará en Turismo, Tecnología, Educación, Emprendimientos y Vacantes</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>29</v>
+      </c>
+      <c r="L37" t="n">
+        <v>500</v>
+      </c>
+      <c r="M37">
+        <f>L37*4</f>
+        <v/>
+      </c>
+      <c r="O37">
+        <f>IF(N37=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q37">
+        <f>IF(N37=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>https://twitter.com/radiopanama/status/1318617982252118016?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="F38" s="1" t="n">
+        <v>44121</v>
+      </c>
+      <c r="G38" s="2" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Entrevista a Juan Mckay sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>30</v>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38">
+        <f>L38*4</f>
+        <v/>
+      </c>
+      <c r="O38">
+        <f>IF(N38=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q38">
+        <f>IF(N38=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA38" t="inlineStr">
+        <is>
+          <t>No Radio Panamá 228 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="F39" s="1" t="n">
+        <v>44121</v>
+      </c>
+      <c r="G39" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>ExpoFeria 2020 se realizará de manera virtual</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>31</v>
+      </c>
+      <c r="L39">
+        <f>IF(N39=3, 750, IF(N39=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M39">
+        <f>L39*4</f>
+        <v/>
+      </c>
+      <c r="O39">
+        <f>IF(N39=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q39">
+        <f>IF(N39=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>https://www.radiopanama.com.pa/noticias/actualidad/expoferia-2020-se-realizara-de-manera-virtual/20201017/nota/4078494.aspx</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="F40" s="1" t="n">
+        <v>44121</v>
+      </c>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>ExpoFeria 2020 se realizará de manera virtual</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>32</v>
+      </c>
+      <c r="L40" t="n">
+        <v>500</v>
+      </c>
+      <c r="M40">
+        <f>L40*4</f>
+        <v/>
+      </c>
+      <c r="O40">
+        <f>IF(N40=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q40">
+        <f>IF(N40=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA40" t="inlineStr">
+        <is>
+          <t>https://twitter.com/radiopanama/status/1317564509284859905?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="F41" s="1" t="n">
+        <v>44119</v>
+      </c>
+      <c r="G41" s="2" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>33</v>
+      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41">
+        <f>L41*4</f>
+        <v/>
+      </c>
+      <c r="O41">
+        <f>IF(N41=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q41">
+        <f>IF(N41=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>No Telemetro 128 segundos</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="F42" s="1" t="n">
+        <v>44119</v>
+      </c>
+      <c r="G42" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>34</v>
+      </c>
+      <c r="L42">
+        <f>IF(N42=3, 750, IF(N42=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M42">
+        <f>L42*4</f>
+        <v/>
+      </c>
+      <c r="O42">
+        <f>IF(N42=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q42">
+        <f>IF(N42=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA42" t="inlineStr">
+        <is>
+          <t>https://www.telemetro.com/nacionales/2020/10/15/expo-feria-asociacion-empresas-panama/3348756.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="F43" s="1" t="n">
+        <v>44119</v>
+      </c>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
+        <v>35</v>
+      </c>
+      <c r="L43" t="n">
+        <v>500</v>
+      </c>
+      <c r="M43">
+        <f>L43*4</f>
+        <v/>
+      </c>
+      <c r="O43">
+        <f>IF(N43=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q43">
+        <f>IF(N43=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA43" t="inlineStr">
+        <is>
+          <t>https://twitter.com/TReporta/status/1316760755795091458?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="F44" s="1" t="n">
+        <v>44120</v>
+      </c>
+      <c r="G44" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K44" t="n">
+        <v>36</v>
+      </c>
+      <c r="L44" t="n">
+        <v>500</v>
+      </c>
+      <c r="M44">
+        <f>L44*4</f>
+        <v/>
+      </c>
+      <c r="O44">
+        <f>IF(N44=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q44">
+        <f>IF(N44=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA44" t="inlineStr">
+        <is>
+          <t>https://twitter.com/TReporta/status/1317004963495673856?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="F45" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G45" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>37</v>
+      </c>
+      <c r="L45" t="n">
+        <v>500</v>
+      </c>
+      <c r="M45">
+        <f>L45*4</f>
+        <v/>
+      </c>
+      <c r="O45">
+        <f>IF(N45=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q45">
+        <f>IF(N45=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>https://twitter.com/TravelPanamaNew/status/1318280935570329611?s=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="F46" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G46" s="2" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K46" t="n">
+        <v>38</v>
+      </c>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46">
+        <f>L46*4</f>
+        <v/>
+      </c>
+      <c r="O46">
+        <f>IF(N46=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q46">
+        <f>IF(N46=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>No NEXTV 245 segundos</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="F47" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G47" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K47" t="n">
+        <v>39</v>
+      </c>
+      <c r="L47">
+        <f>IF(N47=3, 750, IF(N47=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M47">
+        <f>L47*4</f>
+        <v/>
+      </c>
+      <c r="O47">
+        <f>IF(N47=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q47">
+        <f>IF(N47=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=mNC2lC4ALFY</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="F48" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>40</v>
+      </c>
+      <c r="L48">
+        <f>IF(N48=3, 750, IF(N48=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M48">
+        <f>L48*4</f>
+        <v/>
+      </c>
+      <c r="O48">
+        <f>IF(N48=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q48">
+        <f>IF(N48=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t>https://nexnoticias.ruplayers.com/04B6ltCmaHGAfo0/entrevista-a-jaime-carrizo-presidente-de-la-asoc-adedapp.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="F49" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G49" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
+        <v>41</v>
+      </c>
+      <c r="L49">
+        <f>IF(N49=3, 750, IF(N49=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M49">
+        <f>L49*4</f>
+        <v/>
+      </c>
+      <c r="O49">
+        <f>IF(N49=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q49">
+        <f>IF(N49=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>https://pa.domiplay.net/video/entrevista-a-jaime-carrizo-presidente-19-10-20-nex-mnclfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="F50" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G50" s="2" t="inlineStr">
+        <is>
+          <t>Web</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>1 página</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>42</v>
+      </c>
+      <c r="L50">
+        <f>IF(N50=3, 750, IF(N50=1, 1000, ""))</f>
+        <v/>
+      </c>
+      <c r="M50">
+        <f>L50*4</f>
+        <v/>
+      </c>
+      <c r="O50">
+        <f>IF(N50=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q50">
+        <f>IF(N50=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA50" t="inlineStr">
+        <is>
+          <t>https://www.dailymotion.com/video/x7wxvej</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="F51" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G51" s="2" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Entrevista a Juan Mckay sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>43</v>
+      </c>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51">
+        <f>L51*4</f>
+        <v/>
+      </c>
+      <c r="O51">
+        <f>IF(N51=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q51">
+        <f>IF(N51=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t>No TVN 65 segundos</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="F52" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G52" s="2" t="inlineStr">
+        <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>1 post</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Entrevista a Juan Mckay sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K52" t="n">
+        <v>44</v>
+      </c>
+      <c r="L52" t="n">
+        <v>500</v>
+      </c>
+      <c r="M52">
+        <f>L52*4</f>
+        <v/>
+      </c>
+      <c r="O52">
+        <f>IF(N52=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q52">
+        <f>IF(N52=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>https://twitter.com/tvnnoticias/status/1318343401952215040?s=19</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="F53" s="1" t="n">
+        <v>44123</v>
+      </c>
+      <c r="G53" s="2" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K53" t="n">
+        <v>45</v>
+      </c>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53">
+        <f>L53*4</f>
+        <v/>
+      </c>
+      <c r="O53">
+        <f>IF(N53=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q53">
+        <f>IF(N53=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>No ECOTV 60 segundos</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="F54" s="1" t="n">
+        <v>44126</v>
+      </c>
+      <c r="G54" s="2" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Entrevista a Jaime Carrizo, presidente de ADEDAPP, sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+      <c r="K54" t="n">
+        <v>46</v>
+      </c>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54">
+        <f>L54*4</f>
+        <v/>
+      </c>
+      <c r="O54">
+        <f>IF(N54=1,1,"")</f>
+        <v/>
+      </c>
+      <c r="Q54">
+        <f>IF(N54=3,1,"")</f>
+        <v/>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t>No La Exitosa 900 segundos</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Entrevista a Kemmy Almengor sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Entrevista a Kemmy Almengor sobre Expo Feria de la Asociación de Empresas del Área Panamá Pacífico</t>
         </is>
       </c>
     </row>
@@ -1497,6 +2341,31 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G27" r:id="rId19"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G28" r:id="rId20"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G29" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G30" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G31" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G32" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G33" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G34" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G35" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G36" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G37" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G38" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G39" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G40" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G41" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G42" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G43" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G44" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G45" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G46" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G47" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G48" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G49" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G50" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G51" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G52" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G53" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G54" r:id="rId46"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>